<commit_message>
Added a short description on how to use excel.
</commit_message>
<xml_diff>
--- a/Excel/p004-Layers-and-Object.xlsx
+++ b/Excel/p004-Layers-and-Object.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NNfSiX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AEF6DB-4349-4B3D-8A7F-13F10B45B7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E649BF-3C61-4FDA-9092-8A2DD1B1F3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D059B15B-0749-4457-9ACE-2BDFEC19903E}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="layer2" sheetId="10" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="inputX">'p004-Layers-and-Object'!$B$6</definedName>
+    <definedName name="inputX">'p004-Layers-and-Object'!$B$7</definedName>
     <definedName name="output" localSheetId="1">layer1!$LCB$4</definedName>
     <definedName name="output" localSheetId="2">layer2!$LCB$4</definedName>
   </definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>inputs</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Description:</t>
+  </si>
+  <si>
+    <t>double clicking in any cell should update the values</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C6A49B-59EB-4FDD-A744-2E0DA8180E27}">
-  <dimension ref="A2:H24"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,254 +496,259 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" cm="1">
-        <f t="array" ref="B6:E8">{1,2,3,2.5;2,5,-1,2;-1.5,2.7,3.3,-0.8}</f>
+      <c r="B7" cm="1">
+        <f t="array" ref="B7:E9">{1,2,3,2.5;2,5,-1,2;-1.5,2.7,3.3,-0.8}</f>
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>2.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>-1.5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>2.7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>3.3</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>-0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>4</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>5</v>
       </c>
-      <c r="D11" cm="1">
-        <f t="array" ref="D11:G13">_xlfn.ANCHORARRAY(inputX)</f>
+      <c r="D12" cm="1">
+        <f t="array" ref="D12:G14">_xlfn.ANCHORARRAY(inputX)</f>
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>5</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>-1</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14">
         <v>-1.5</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>2.7</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>3.3</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D17" cm="1">
-        <f t="array" aca="1" ref="D17:H19" ca="1">_xlfn.ANCHORARRAY(layer1!output)</f>
-        <v>-0.76874574266925599</v>
-      </c>
-      <c r="E17">
-        <f ca="1"/>
-        <v>-2.0042683643349903</v>
-      </c>
-      <c r="F17">
-        <f ca="1"/>
-        <v>-1.6187704646209942</v>
-      </c>
-      <c r="G17">
-        <f ca="1"/>
-        <v>0.40248077271631377</v>
-      </c>
-      <c r="H17">
-        <f ca="1"/>
-        <v>1.5612332965891988</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <f ca="1"/>
-        <v>-0.12785404298746372</v>
+      <c r="D18" cm="1">
+        <f t="array" aca="1" ref="D18:H20" ca="1">_xlfn.ANCHORARRAY(layer1!output)</f>
+        <v>-1.3389166781346</v>
       </c>
       <c r="E18">
         <f ca="1"/>
-        <v>3.840258858702239</v>
+        <v>2.3598235729837533</v>
       </c>
       <c r="F18">
         <f ca="1"/>
-        <v>1.9957749869250823</v>
+        <v>-3.5687938497053313</v>
       </c>
       <c r="G18">
         <f ca="1"/>
-        <v>1.7539210535656427</v>
+        <v>-1.1502032779993099</v>
       </c>
       <c r="H18">
         <f ca="1"/>
-        <v>4.1451648359949678</v>
+        <v>2.4032639837563221</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
       <c r="D19">
         <f ca="1"/>
-        <v>-2.9536554801986568</v>
+        <v>-5.258531897143504</v>
       </c>
       <c r="E19">
         <f ca="1"/>
-        <v>-0.31152717023104703</v>
+        <v>-0.72920326598116558</v>
       </c>
       <c r="F19">
         <f ca="1"/>
-        <v>-0.96771705663060636</v>
+        <v>-5.3351345627902189</v>
       </c>
       <c r="G19">
         <f ca="1"/>
-        <v>-0.51300028515799212</v>
+        <v>1.8736831093142843</v>
       </c>
       <c r="H19">
         <f ca="1"/>
-        <v>-1.5683618323627797</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>4.3781663970635281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20">
+        <f ca="1"/>
+        <v>3.9261584376876062</v>
+      </c>
+      <c r="E20">
+        <f ca="1"/>
+        <v>8.0318021195703304E-2</v>
+      </c>
+      <c r="F20">
+        <f ca="1"/>
+        <v>-1.2380363365887603</v>
+      </c>
+      <c r="G20">
+        <f ca="1"/>
+        <v>-0.83027734614832105</v>
+      </c>
+      <c r="H20">
+        <f ca="1"/>
+        <v>-0.26385002317793438</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B22" cm="1">
-        <f t="array" aca="1" ref="B22:C24" ca="1">_xlfn.ANCHORARRAY(layer2!output)</f>
-        <v>-2.4243792104586981</v>
-      </c>
-      <c r="C22">
-        <f ca="1"/>
-        <v>-3.3438685939472852</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <f ca="1"/>
-        <v>2.115599505699957</v>
+      <c r="B23" cm="1">
+        <f t="array" aca="1" ref="B23:C25" ca="1">_xlfn.ANCHORARRAY(layer2!output)</f>
+        <v>0.67033443073072529</v>
       </c>
       <c r="C23">
         <f ca="1"/>
-        <v>0.4910694838996279</v>
+        <v>-3.3089702464212651</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <f ca="1"/>
-        <v>2.0620661787066106</v>
+        <v>-2.0362424380896962</v>
       </c>
       <c r="C24">
         <f ca="1"/>
-        <v>-0.72943062588029028</v>
+        <v>-3.8215746697706443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f ca="1"/>
+        <v>2.9921305134978202</v>
+      </c>
+      <c r="C25">
+        <f ca="1"/>
+        <v>0.32412372915236498</v>
       </c>
     </row>
   </sheetData>
@@ -799,23 +807,23 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3:F6" ca="1">_xlfn.RANDARRAY($B$2,$C$2,-1,1)</f>
-        <v>0.62002105121425388</v>
+        <v>-0.93660423905676704</v>
       </c>
       <c r="C3">
         <f ca="1"/>
-        <v>-0.51483705442840955</v>
+        <v>-0.22769171247218001</v>
       </c>
       <c r="D3">
         <f ca="1"/>
-        <v>-0.66857996875795123</v>
+        <v>-0.64476268523163283</v>
       </c>
       <c r="E3">
         <f ca="1"/>
-        <v>7.0221123494929927E-2</v>
+        <v>-0.65676145507415495</v>
       </c>
       <c r="F3">
         <f ca="1"/>
-        <v>0.76876917175528137</v>
+        <v>-2.5425438848975412E-2</v>
       </c>
       <c r="LCA3" t="s">
         <v>3</v>
@@ -844,130 +852,130 @@
     <row r="4" spans="1:6 8191:8198" x14ac:dyDescent="0.25">
       <c r="B4">
         <f ca="1"/>
-        <v>-0.36709055298548887</v>
+        <v>-0.19024209897286193</v>
       </c>
       <c r="C4">
         <f ca="1"/>
-        <v>0.79398350326681144</v>
+        <v>-0.31182873245422926</v>
       </c>
       <c r="D4">
         <f ca="1"/>
-        <v>0.37549337830151863</v>
+        <v>-0.69458808424214213</v>
       </c>
       <c r="E4">
         <f ca="1"/>
-        <v>0.18252724806912513</v>
+        <v>0.33087679080164589</v>
       </c>
       <c r="F4">
         <f ca="1"/>
-        <v>0.30411240844765319</v>
+        <v>0.47237981087867098</v>
       </c>
       <c r="LCA4" t="s">
         <v>2</v>
       </c>
       <c r="LCB4" cm="1">
         <f t="array" aca="1" ref="LCB4:LCF6" ca="1">(MMULT(INDIRECT("'p004-Layers-and-Object'!D"&amp;MATCH($A$2,'p004-Layers-and-Object'!A:A,0)&amp;"#"),_xlfn.ANCHORARRAY(B3)))+(_xlfn.ANCHORARRAY(LCB3))</f>
-        <v>-0.76874574266925599</v>
+        <v>-1.3389166781346</v>
       </c>
       <c r="LCC4">
         <f ca="1"/>
-        <v>-2.0042683643349903</v>
+        <v>2.3598235729837533</v>
       </c>
       <c r="LCD4">
         <f ca="1"/>
-        <v>-1.6187704646209942</v>
+        <v>-3.5687938497053313</v>
       </c>
       <c r="LCE4">
         <f ca="1"/>
-        <v>0.40248077271631377</v>
+        <v>-1.1502032779993099</v>
       </c>
       <c r="LCF4">
         <f ca="1"/>
-        <v>1.5612332965891988</v>
+        <v>2.4032639837563221</v>
       </c>
     </row>
     <row r="5" spans="1:6 8191:8198" x14ac:dyDescent="0.25">
       <c r="B5">
         <f ca="1"/>
-        <v>-0.29153681465926429</v>
+        <v>0.71077950919410982</v>
       </c>
       <c r="C5">
         <f ca="1"/>
-        <v>-0.98880414834622488</v>
+        <v>0.37753364089916852</v>
       </c>
       <c r="D5">
         <f ca="1"/>
-        <v>-0.82835583379595756</v>
+        <v>-0.19271036049273205</v>
       </c>
       <c r="E5">
         <f ca="1"/>
-        <v>-0.21384660110695597</v>
+        <v>-0.7226407026697419</v>
       </c>
       <c r="F5">
         <f ca="1"/>
-        <v>-0.27637441291036757</v>
+        <v>-0.25881599402639988</v>
       </c>
       <c r="LCB5">
         <f ca="1"/>
-        <v>-0.12785404298746372</v>
+        <v>-5.258531897143504</v>
       </c>
       <c r="LCC5">
         <f ca="1"/>
-        <v>3.840258858702239</v>
+        <v>-0.72920326598116558</v>
       </c>
       <c r="LCD5">
         <f ca="1"/>
-        <v>1.9957749869250823</v>
+        <v>-5.3351345627902189</v>
       </c>
       <c r="LCE5">
         <f ca="1"/>
-        <v>1.7539210535656427</v>
+        <v>1.8736831093142843</v>
       </c>
       <c r="LCF5">
         <f ca="1"/>
-        <v>4.1451648359949678</v>
+        <v>4.3781663970635281</v>
       </c>
     </row>
     <row r="6" spans="1:6 8191:8198" x14ac:dyDescent="0.25">
       <c r="B6">
         <f ca="1"/>
-        <v>8.8009902426104292E-2</v>
+        <v>-0.86166670748577556</v>
       </c>
       <c r="C6">
         <f ca="1"/>
-        <v>-4.4394348560611752E-2</v>
+        <v>0.83142873106675452</v>
       </c>
       <c r="D6">
         <f ca="1"/>
-        <v>0.31355609956871699</v>
+        <v>-0.38268956580448732</v>
       </c>
       <c r="E6">
         <f ca="1"/>
-        <v>0.2434979825616006</v>
+        <v>0.40509068139231141</v>
       </c>
       <c r="F6">
         <f ca="1"/>
-        <v>0.40534501866788553</v>
+        <v>0.90415111317086216</v>
       </c>
       <c r="LCB6">
         <f ca="1"/>
-        <v>-2.9536554801986568</v>
+        <v>3.9261584376876062</v>
       </c>
       <c r="LCC6">
         <f ca="1"/>
-        <v>-0.31152717023104703</v>
+        <v>8.0318021195703304E-2</v>
       </c>
       <c r="LCD6">
         <f ca="1"/>
-        <v>-0.96771705663060636</v>
+        <v>-1.2380363365887603</v>
       </c>
       <c r="LCE6">
         <f ca="1"/>
-        <v>-0.51300028515799212</v>
+        <v>-0.83027734614832105</v>
       </c>
       <c r="LCF6">
         <f ca="1"/>
-        <v>-1.5683618323627797</v>
+        <v>-0.26385002317793438</v>
       </c>
     </row>
   </sheetData>
@@ -1024,11 +1032,11 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3:C7" ca="1">_xlfn.RANDARRAY($B$2,$C$2,-1,1)</f>
-        <v>-0.67440778826778991</v>
+        <v>0.89332399802965456</v>
       </c>
       <c r="C3">
         <f ca="1"/>
-        <v>0.48845165954648939</v>
+        <v>0.28249032963831011</v>
       </c>
       <c r="LCA3" t="s">
         <v>3</v>
@@ -1045,68 +1053,68 @@
     <row r="4" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B4">
         <f ca="1"/>
-        <v>0.81045809113109679</v>
+        <v>0.25875352810845875</v>
       </c>
       <c r="C4">
         <f ca="1"/>
-        <v>0.74990821302088784</v>
+        <v>-0.60907258837737444</v>
       </c>
       <c r="LCA4" t="s">
         <v>2</v>
       </c>
       <c r="LCB4" cm="1">
         <f t="array" aca="1" ref="LCB4:LCC6" ca="1">(MMULT(INDIRECT("'p004-Layers-and-Object'!D"&amp;MATCH($A$2,'p004-Layers-and-Object'!A:A,0)&amp;"#"),_xlfn.ANCHORARRAY(B3)))+(_xlfn.ANCHORARRAY(LCB3))</f>
-        <v>-2.4243792104586981</v>
+        <v>0.67033443073072529</v>
       </c>
       <c r="LCC4">
         <f ca="1"/>
-        <v>-3.3438685939472852</v>
+        <v>-3.3089702464212651</v>
       </c>
     </row>
     <row r="5" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B5">
         <f ca="1"/>
-        <v>0.38758428332607808</v>
+        <v>0.19470593387391411</v>
       </c>
       <c r="C5">
         <f ca="1"/>
-        <v>0.17362524188731299</v>
+        <v>0.67793714283827011</v>
       </c>
       <c r="LCB5">
         <f ca="1"/>
-        <v>2.115599505699957</v>
+        <v>-2.0362424380896962</v>
       </c>
       <c r="LCC5">
         <f ca="1"/>
-        <v>0.4910694838996279</v>
+        <v>-3.8215746697706443</v>
       </c>
     </row>
     <row r="6" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B6">
         <f ca="1"/>
-        <v>-3.176668711050068E-2</v>
+        <v>8.4437976146512161E-2</v>
       </c>
       <c r="C6">
         <f ca="1"/>
-        <v>0.68806377536086849</v>
+        <v>-0.21422080172868063</v>
       </c>
       <c r="LCB6">
         <f ca="1"/>
-        <v>2.0620661787066106</v>
+        <v>2.9921305134978202</v>
       </c>
       <c r="LCC6">
         <f ca="1"/>
-        <v>-0.72943062588029028</v>
+        <v>0.32412372915236498</v>
       </c>
     </row>
     <row r="7" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B7">
         <f ca="1"/>
-        <v>-0.43443625251044948</v>
+        <v>0.85208880320689473</v>
       </c>
       <c r="C7">
         <f ca="1"/>
-        <v>-0.93594543644197836</v>
+        <v>0.28277586695916113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated short description to be correct.
</commit_message>
<xml_diff>
--- a/Excel/p004-Layers-and-Object.xlsx
+++ b/Excel/p004-Layers-and-Object.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NNfSiX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E649BF-3C61-4FDA-9092-8A2DD1B1F3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B41934-16D6-493A-A514-9180743A8EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D059B15B-0749-4457-9ACE-2BDFEC19903E}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>n_neurons</t>
   </si>
   <si>
-    <t>for each layer create a new sheet and rename it to the name of the variable.</t>
-  </si>
-  <si>
     <t>for the output of the layer use layerX!output#</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>double clicking in any cell should update the values</t>
+  </si>
+  <si>
+    <t>for each layer copy an existing layer sheet and rename it to the name of the variable.</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,22 +491,22 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -654,68 +654,68 @@
       </c>
       <c r="D18" cm="1">
         <f t="array" aca="1" ref="D18:H20" ca="1">_xlfn.ANCHORARRAY(layer1!output)</f>
-        <v>-1.3389166781346</v>
+        <v>1.7135638802948396</v>
       </c>
       <c r="E18">
         <f ca="1"/>
-        <v>2.3598235729837533</v>
+        <v>-2.3233390021035683</v>
       </c>
       <c r="F18">
         <f ca="1"/>
-        <v>-3.5687938497053313</v>
+        <v>3.3561747038237009</v>
       </c>
       <c r="G18">
         <f ca="1"/>
-        <v>-1.1502032779993099</v>
+        <v>0.13067180937102751</v>
       </c>
       <c r="H18">
         <f ca="1"/>
-        <v>2.4032639837563221</v>
+        <v>1.4737931148461889</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D19">
         <f ca="1"/>
-        <v>-5.258531897143504</v>
+        <v>-0.75816435131366577</v>
       </c>
       <c r="E19">
         <f ca="1"/>
-        <v>-0.72920326598116558</v>
+        <v>1.5922104364376704</v>
       </c>
       <c r="F19">
         <f ca="1"/>
-        <v>-5.3351345627902189</v>
+        <v>-0.73330099529160231</v>
       </c>
       <c r="G19">
         <f ca="1"/>
-        <v>1.8736831093142843</v>
+        <v>2.9661618257564655</v>
       </c>
       <c r="H19">
         <f ca="1"/>
-        <v>4.3781663970635281</v>
+        <v>-2.1456905423563075</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20">
         <f ca="1"/>
-        <v>3.9261584376876062</v>
+        <v>2.2250712760903335</v>
       </c>
       <c r="E20">
         <f ca="1"/>
-        <v>8.0318021195703304E-2</v>
+        <v>-4.781838625555566</v>
       </c>
       <c r="F20">
         <f ca="1"/>
-        <v>-1.2380363365887603</v>
+        <v>-0.2314473815002912</v>
       </c>
       <c r="G20">
         <f ca="1"/>
-        <v>-0.83027734614832105</v>
+        <v>1.373695261248955</v>
       </c>
       <c r="H20">
         <f ca="1"/>
-        <v>-0.26385002317793438</v>
+        <v>1.1141175093502376</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -724,31 +724,31 @@
       </c>
       <c r="B23" cm="1">
         <f t="array" aca="1" ref="B23:C25" ca="1">_xlfn.ANCHORARRAY(layer2!output)</f>
-        <v>0.67033443073072529</v>
+        <v>0.79275573093774376</v>
       </c>
       <c r="C23">
         <f ca="1"/>
-        <v>-3.3089702464212651</v>
+        <v>1.6522262163917723E-3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <f ca="1"/>
-        <v>-2.0362424380896962</v>
+        <v>-1.1644819883067308</v>
       </c>
       <c r="C24">
         <f ca="1"/>
-        <v>-3.8215746697706443</v>
+        <v>-0.30115229968564672</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25">
         <f ca="1"/>
-        <v>2.9921305134978202</v>
+        <v>0.45486572112788665</v>
       </c>
       <c r="C25">
         <f ca="1"/>
-        <v>0.32412372915236498</v>
+        <v>-0.23480064538132531</v>
       </c>
     </row>
   </sheetData>
@@ -807,23 +807,23 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3:F6" ca="1">_xlfn.RANDARRAY($B$2,$C$2,-1,1)</f>
-        <v>-0.93660423905676704</v>
+        <v>-0.80310009812573946</v>
       </c>
       <c r="C3">
         <f ca="1"/>
-        <v>-0.22769171247218001</v>
+        <v>0.60895652225939401</v>
       </c>
       <c r="D3">
         <f ca="1"/>
-        <v>-0.64476268523163283</v>
+        <v>0.48540830287631165</v>
       </c>
       <c r="E3">
         <f ca="1"/>
-        <v>-0.65676145507415495</v>
+        <v>0.70932291854793639</v>
       </c>
       <c r="F3">
         <f ca="1"/>
-        <v>-2.5425438848975412E-2</v>
+        <v>0.22255667683846636</v>
       </c>
       <c r="LCA3" t="s">
         <v>3</v>
@@ -852,130 +852,130 @@
     <row r="4" spans="1:6 8191:8198" x14ac:dyDescent="0.25">
       <c r="B4">
         <f ca="1"/>
-        <v>-0.19024209897286193</v>
+        <v>4.8119354015681237E-2</v>
       </c>
       <c r="C4">
         <f ca="1"/>
-        <v>-0.31182873245422926</v>
+        <v>-0.18402246738659067</v>
       </c>
       <c r="D4">
         <f ca="1"/>
-        <v>-0.69458808424214213</v>
+        <v>-0.47333814949992825</v>
       </c>
       <c r="E4">
         <f ca="1"/>
-        <v>0.33087679080164589</v>
+        <v>0.62782505641739461</v>
       </c>
       <c r="F4">
         <f ca="1"/>
-        <v>0.47237981087867098</v>
+        <v>-0.34894173953608876</v>
       </c>
       <c r="LCA4" t="s">
         <v>2</v>
       </c>
       <c r="LCB4" cm="1">
         <f t="array" aca="1" ref="LCB4:LCF6" ca="1">(MMULT(INDIRECT("'p004-Layers-and-Object'!D"&amp;MATCH($A$2,'p004-Layers-and-Object'!A:A,0)&amp;"#"),_xlfn.ANCHORARRAY(B3)))+(_xlfn.ANCHORARRAY(LCB3))</f>
-        <v>-1.3389166781346</v>
+        <v>1.7135638802948396</v>
       </c>
       <c r="LCC4">
         <f ca="1"/>
-        <v>2.3598235729837533</v>
+        <v>-2.3233390021035683</v>
       </c>
       <c r="LCD4">
         <f ca="1"/>
-        <v>-3.5687938497053313</v>
+        <v>3.3561747038237009</v>
       </c>
       <c r="LCE4">
         <f ca="1"/>
-        <v>-1.1502032779993099</v>
+        <v>0.13067180937102751</v>
       </c>
       <c r="LCF4">
         <f ca="1"/>
-        <v>2.4032639837563221</v>
+        <v>1.4737931148461889</v>
       </c>
     </row>
     <row r="5" spans="1:6 8191:8198" x14ac:dyDescent="0.25">
       <c r="B5">
         <f ca="1"/>
-        <v>0.71077950919410982</v>
+        <v>0.39085327689763716</v>
       </c>
       <c r="C5">
         <f ca="1"/>
-        <v>0.37753364089916852</v>
+        <v>-0.98406182368342954</v>
       </c>
       <c r="D5">
         <f ca="1"/>
-        <v>-0.19271036049273205</v>
+        <v>0.70334735691246508</v>
       </c>
       <c r="E5">
         <f ca="1"/>
-        <v>-0.7226407026697419</v>
+        <v>3.6520092887359246E-2</v>
       </c>
       <c r="F5">
         <f ca="1"/>
-        <v>-0.25881599402639988</v>
+        <v>0.70746798000491662</v>
       </c>
       <c r="LCB5">
         <f ca="1"/>
-        <v>-5.258531897143504</v>
+        <v>-0.75816435131366577</v>
       </c>
       <c r="LCC5">
         <f ca="1"/>
-        <v>-0.72920326598116558</v>
+        <v>1.5922104364376704</v>
       </c>
       <c r="LCD5">
         <f ca="1"/>
-        <v>-5.3351345627902189</v>
+        <v>-0.73330099529160231</v>
       </c>
       <c r="LCE5">
         <f ca="1"/>
-        <v>1.8736831093142843</v>
+        <v>2.9661618257564655</v>
       </c>
       <c r="LCF5">
         <f ca="1"/>
-        <v>4.3781663970635281</v>
+        <v>-2.1456905423563075</v>
       </c>
     </row>
     <row r="6" spans="1:6 8191:8198" x14ac:dyDescent="0.25">
       <c r="B6">
         <f ca="1"/>
-        <v>-0.86166670748577556</v>
+        <v>0.49914617587852206</v>
       </c>
       <c r="C6">
         <f ca="1"/>
-        <v>0.83142873106675452</v>
+        <v>0.15517395258420308</v>
       </c>
       <c r="D6">
         <f ca="1"/>
-        <v>-0.38268956580448732</v>
+        <v>0.68296025168394014</v>
       </c>
       <c r="E6">
         <f ca="1"/>
-        <v>0.40509068139231141</v>
+        <v>-0.77754460026951033</v>
       </c>
       <c r="F6">
         <f ca="1"/>
-        <v>0.90415111317086216</v>
+        <v>-6.9313609173939916E-2</v>
       </c>
       <c r="LCB6">
         <f ca="1"/>
-        <v>3.9261584376876062</v>
+        <v>2.2250712760903335</v>
       </c>
       <c r="LCC6">
         <f ca="1"/>
-        <v>8.0318021195703304E-2</v>
+        <v>-4.781838625555566</v>
       </c>
       <c r="LCD6">
         <f ca="1"/>
-        <v>-1.2380363365887603</v>
+        <v>-0.2314473815002912</v>
       </c>
       <c r="LCE6">
         <f ca="1"/>
-        <v>-0.83027734614832105</v>
+        <v>1.373695261248955</v>
       </c>
       <c r="LCF6">
         <f ca="1"/>
-        <v>-0.26385002317793438</v>
+        <v>1.1141175093502376</v>
       </c>
     </row>
   </sheetData>
@@ -1032,11 +1032,11 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3:C7" ca="1">_xlfn.RANDARRAY($B$2,$C$2,-1,1)</f>
-        <v>0.89332399802965456</v>
+        <v>-0.11065363356677227</v>
       </c>
       <c r="C3">
         <f ca="1"/>
-        <v>0.28249032963831011</v>
+        <v>-0.38718773090308578</v>
       </c>
       <c r="LCA3" t="s">
         <v>3</v>
@@ -1053,68 +1053,68 @@
     <row r="4" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B4">
         <f ca="1"/>
-        <v>0.25875352810845875</v>
+        <v>-0.22368228478168839</v>
       </c>
       <c r="C4">
         <f ca="1"/>
-        <v>-0.60907258837737444</v>
+        <v>-9.4782865230381264E-2</v>
       </c>
       <c r="LCA4" t="s">
         <v>2</v>
       </c>
       <c r="LCB4" cm="1">
         <f t="array" aca="1" ref="LCB4:LCC6" ca="1">(MMULT(INDIRECT("'p004-Layers-and-Object'!D"&amp;MATCH($A$2,'p004-Layers-and-Object'!A:A,0)&amp;"#"),_xlfn.ANCHORARRAY(B3)))+(_xlfn.ANCHORARRAY(LCB3))</f>
-        <v>0.67033443073072529</v>
+        <v>0.79275573093774376</v>
       </c>
       <c r="LCC4">
         <f ca="1"/>
-        <v>-3.3089702464212651</v>
+        <v>1.6522262163917723E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B5">
         <f ca="1"/>
-        <v>0.19470593387391411</v>
+        <v>0.14169999298613489</v>
       </c>
       <c r="C5">
         <f ca="1"/>
-        <v>0.67793714283827011</v>
+        <v>5.5157054424766816E-2</v>
       </c>
       <c r="LCB5">
         <f ca="1"/>
-        <v>-2.0362424380896962</v>
+        <v>-1.1644819883067308</v>
       </c>
       <c r="LCC5">
         <f ca="1"/>
-        <v>-3.8215746697706443</v>
+        <v>-0.30115229968564672</v>
       </c>
     </row>
     <row r="6" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B6">
         <f ca="1"/>
-        <v>8.4437976146512161E-2</v>
+        <v>-0.25569802393763408</v>
       </c>
       <c r="C6">
         <f ca="1"/>
-        <v>-0.21422080172868063</v>
+        <v>-7.9553931036118186E-3</v>
       </c>
       <c r="LCB6">
         <f ca="1"/>
-        <v>2.9921305134978202</v>
+        <v>0.45486572112788665</v>
       </c>
       <c r="LCC6">
         <f ca="1"/>
-        <v>0.32412372915236498</v>
+        <v>-0.23480064538132531</v>
       </c>
     </row>
     <row r="7" spans="1:3 8191:8198" x14ac:dyDescent="0.25">
       <c r="B7">
         <f ca="1"/>
-        <v>0.85208880320689473</v>
+        <v>1.3923674612103198E-2</v>
       </c>
       <c r="C7">
         <f ca="1"/>
-        <v>0.28277586695916113</v>
+        <v>0.17698090827684831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>